<commit_message>
Work on 3_InterRaterReliab.R script. Added Gwet's AC calculation.
</commit_message>
<xml_diff>
--- a/data/ecology/Mel/002.xlsx
+++ b/data/ecology/Mel/002.xlsx
@@ -11348,10 +11348,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36965efa-5a39-45c9-9312-a4f852bee1e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39724199-8FDF-46B3-95BE-67B77A5FD1AB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC8C5A80-95CD-41AF-88D9-2274ED8C77B1}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7425A53-730C-4797-A789-3CBC98628F3C}"/>
 </file>
</xml_diff>